<commit_message>
Added chrome driver & smoke clear data sheet
Signed-off-by: Vineet <automationnavatar@gmail.com>
</commit_message>
<xml_diff>
--- a/SmokeTestCases.xlsx
+++ b/SmokeTestCases.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView tabRatio="587" windowHeight="11160" windowWidth="20730" xWindow="-120" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="587"/>
   </bookViews>
   <sheets>
-    <sheet name="FilePath" r:id="rId1" sheetId="2"/>
-    <sheet name="Institutions" r:id="rId2" sheetId="3"/>
-    <sheet name="Limited Partner" r:id="rId3" sheetId="11"/>
-    <sheet name="Contact" r:id="rId4" sheetId="4"/>
-    <sheet name="Funds" r:id="rId5" sheetId="5"/>
-    <sheet name="Fundraisings" r:id="rId6" sheetId="6"/>
-    <sheet name="Partnerships" r:id="rId7" sheetId="12"/>
-    <sheet name="Commitments" r:id="rId8" sheetId="13"/>
-    <sheet name="Users" r:id="rId9" sheetId="8"/>
-    <sheet name="FolderTemp" r:id="rId10" sheetId="7"/>
-    <sheet name="DR Analytics" r:id="rId11" sheetId="9"/>
-    <sheet name="SpecialChar" r:id="rId12" sheetId="10"/>
+    <sheet name="FilePath" sheetId="2" r:id="rId1"/>
+    <sheet name="Institutions" sheetId="3" r:id="rId2"/>
+    <sheet name="Limited Partner" sheetId="11" r:id="rId3"/>
+    <sheet name="Contact" sheetId="4" r:id="rId4"/>
+    <sheet name="Funds" sheetId="5" r:id="rId5"/>
+    <sheet name="Fundraisings" sheetId="6" r:id="rId6"/>
+    <sheet name="Partnerships" sheetId="12" r:id="rId7"/>
+    <sheet name="Commitments" sheetId="13" r:id="rId8"/>
+    <sheet name="Users" sheetId="8" r:id="rId9"/>
+    <sheet name="FolderTemp" sheetId="7" r:id="rId10"/>
+    <sheet name="DR Analytics" sheetId="9" r:id="rId11"/>
+    <sheet name="SpecialChar" sheetId="10" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="339">
   <si>
     <t>Internal</t>
   </si>
@@ -947,12 +947,6 @@
     <t>CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log</t>
   </si>
   <si>
-    <t>SharedFile1.pdf&lt;break&gt;SharedFile2.xlsx&lt;break&gt;SharedFile3.log</t>
-  </si>
-  <si>
-    <t>StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log</t>
-  </si>
-  <si>
     <t>Smoketc012_2_updateDocumentCRMSideAndCheckDuplicatePopUp</t>
   </si>
   <si>
@@ -971,9 +965,6 @@
     <t>Smoketc030_2_updateDocumentCRMSideAndCheckDuplicatePopUp</t>
   </si>
   <si>
-    <t>Onlineimport.log&lt;break&gt;Onlineimport.xlsx&lt;break&gt;OnlineimportFile1.pdf&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log</t>
-  </si>
-  <si>
     <t>SmokeTemplate</t>
   </si>
   <si>
@@ -1025,84 +1016,15 @@
     <t>AAAP1</t>
   </si>
   <si>
-    <t>automationnavatar+89473@gmail.com</t>
-  </si>
-  <si>
-    <t>automationnavatar+61382@gmail.com</t>
-  </si>
-  <si>
-    <t>CMT - 002848</t>
-  </si>
-  <si>
-    <t>CMT - 002849</t>
-  </si>
-  <si>
-    <t>CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log</t>
-  </si>
-  <si>
-    <t>CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log</t>
-  </si>
-  <si>
-    <t>SharedFile1.pdf&lt;break&gt;SharedFile2.xlsx&lt;break&gt;SharedFile3.log&lt;break&gt;SharedFile1.pdf&lt;break&gt;SharedFile2.xlsx&lt;break&gt;SharedFile3.log&lt;break&gt;SharedFile1.pdf&lt;break&gt;SharedFile2.xlsx&lt;break&gt;SharedFile3.log&lt;break&gt;SharedFile1.pdf&lt;break&gt;SharedFile2.xlsx&lt;break&gt;SharedFile3.log</t>
-  </si>
-  <si>
-    <t>StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log</t>
-  </si>
-  <si>
-    <t>CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log</t>
-  </si>
-  <si>
-    <t>automationnavatar+68493@gmail.com</t>
-  </si>
-  <si>
-    <t>navatariptesting+51753@gmail.com</t>
-  </si>
-  <si>
-    <t>User19353</t>
-  </si>
-  <si>
-    <t>User6874</t>
-  </si>
-  <si>
-    <t>navatariptesting+88869@gmail.com</t>
-  </si>
-  <si>
-    <t>User81019</t>
-  </si>
-  <si>
-    <t>navatariptesting+60456@gmail.com</t>
-  </si>
-  <si>
     <t>petrial4440</t>
   </si>
   <si>
-    <t>automationnavatar+13150@gmail.com</t>
-  </si>
-  <si>
-    <t>automationnavatar+35014@gmail.com</t>
-  </si>
-  <si>
-    <t>automationnavatar+3670@gmail.com</t>
-  </si>
-  <si>
     <t>CMT - 000932</t>
   </si>
   <si>
     <t>CMT - 000933</t>
   </si>
   <si>
-    <t>CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log</t>
-  </si>
-  <si>
-    <t>SharedFile1.pdf&lt;break&gt;SharedFile2.xlsx&lt;break&gt;SharedFile3.log&lt;break&gt;SharedFile1.pdf&lt;break&gt;SharedFile2.xlsx&lt;break&gt;SharedFile3.log&lt;break&gt;SharedFile1.pdf&lt;break&gt;SharedFile2.xlsx&lt;break&gt;SharedFile3.log&lt;break&gt;SharedFile1.pdf&lt;break&gt;SharedFile2.xlsx&lt;break&gt;SharedFile3.log&lt;break&gt;SharedFile1.pdf&lt;break&gt;SharedFile2.xlsx&lt;break&gt;SharedFile3.log</t>
-  </si>
-  <si>
-    <t>StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log</t>
-  </si>
-  <si>
-    <t>CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log</t>
-  </si>
-  <si>
     <t>CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log</t>
   </si>
   <si>
@@ -1112,32 +1034,25 @@
     <t>http://track.smtpsendemail.com/437921/c?p=qiAU-YIpGi0vpff7CdWNuiTxpKRNZg-z4DdHz_XHFo7EGbWyQK-dygHpcUEtjiabiVKG2PAbsbn6QICLngfRP1VMS9qS6k833gXYlgPbQbnwJE9FCFioQavCqOEIVFZFGM6_DYu4fB1LeKOkMF5BIFOKKt6_rU3ZzIg0Xmn-WnQ0m9EQSzbjDGZHnE4U0QNjU8udDRmsSlaAdU13i-mJ8g==</t>
   </si>
   <si>
-    <t>SharedFile1.pdf&lt;break&gt;SharedFile2.xlsx&lt;break&gt;SharedFile3.log&lt;break&gt;SharedFile1.pdf&lt;break&gt;SharedFile2.xlsx&lt;break&gt;SharedFile3.log</t>
-  </si>
-  <si>
     <t>StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log</t>
   </si>
   <si>
-    <t>CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log</t>
-  </si>
-  <si>
     <t>CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log</t>
   </si>
   <si>
-    <t>Onlineimport.log&lt;break&gt;Onlineimport.xlsx&lt;break&gt;OnlineimportFile1.pdf&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log</t>
-  </si>
-  <si>
     <t>Onlineimport.log&lt;break&gt;Onlineimport.xlsx&lt;break&gt;OnlineimportFile1.pdf&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log</t>
   </si>
   <si>
     <t>http://dtaghub03.secure.force.com/apex/ResetPassword?userId=MDA1NmcwMDAwMDVBbGlGQUFT</t>
+  </si>
+  <si>
+    <t>User</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1233,78 +1148,78 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="33">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="1"/>
-    <xf applyBorder="1" applyFill="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1321,10 +1236,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1359,7 +1274,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1394,7 +1309,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1488,21 +1403,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1519,7 +1434,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1571,48 +1486,48 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK105"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AJ105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="65.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="103.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="57.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="53.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="103.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="255.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="115.5703125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="46.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="33.42578125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="52.7109375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="224.140625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="209.28515625" collapsed="true"/>
+    <col min="1" max="1" width="65.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="103.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="57.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="53.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="103.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="255.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="115.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="46.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="33.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="52.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="224.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="209.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>95</v>
       </c>
@@ -1730,7 +1645,7 @@
         <v>2</v>
       </c>
     </row>
-    <row ht="15.75" r="3" spans="1:36" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>257</v>
       </c>
@@ -1738,7 +1653,7 @@
         <v>217</v>
       </c>
     </row>
-    <row customFormat="1" ht="15.75" r="4" s="7" spans="1:36" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>259</v>
       </c>
@@ -1770,15 +1685,6 @@
       <c r="E6" t="s">
         <v>2</v>
       </c>
-      <c r="F6" t="s">
-        <v>353</v>
-      </c>
-      <c r="H6" t="s">
-        <v>354</v>
-      </c>
-      <c r="I6" t="s">
-        <v>355</v>
-      </c>
       <c r="J6" t="s">
         <v>304</v>
       </c>
@@ -1799,7 +1705,7 @@
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E8" t="s">
         <v>2</v>
@@ -1810,7 +1716,7 @@
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B9" t="s">
         <v>215</v>
@@ -1819,13 +1725,13 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>357</v>
+        <v>331</v>
       </c>
       <c r="I9" t="s">
         <v>266</v>
       </c>
       <c r="J9" t="s">
-        <v>358</v>
+        <v>332</v>
       </c>
       <c r="N9" t="s">
         <v>267</v>
@@ -1935,15 +1841,6 @@
       <c r="E18" t="s">
         <v>2</v>
       </c>
-      <c r="F18" t="s">
-        <v>309</v>
-      </c>
-      <c r="H18" t="s">
-        <v>360</v>
-      </c>
-      <c r="I18" t="s">
-        <v>361</v>
-      </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
@@ -1961,7 +1858,7 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E20" t="s">
         <v>2</v>
@@ -1972,7 +1869,7 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B21" t="s">
         <v>215</v>
@@ -1981,16 +1878,16 @@
         <v>2</v>
       </c>
       <c r="F21" t="s">
-        <v>363</v>
+        <v>335</v>
       </c>
       <c r="I21" t="s">
-        <v>365</v>
+        <v>336</v>
       </c>
       <c r="J21" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="M21" t="s">
-        <v>361</v>
+        <v>334</v>
       </c>
       <c r="N21" t="s">
         <v>267</v>
@@ -2094,7 +1991,7 @@
         <v>303</v>
       </c>
       <c r="AE28" s="7" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
@@ -2326,13 +2223,13 @@
       <c r="A105" s="3"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
@@ -2340,25 +2237,25 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="77.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="5" max="10" width="9.140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="9.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="255.7109375" collapsed="true"/>
-    <col min="13" max="16384" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="77.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="10" width="9.140625" collapsed="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="255.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="9.140625" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>213</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row customFormat="1" r="2" s="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -2453,14 +2350,14 @@
       <c r="L8" s="22"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
@@ -2468,9 +2365,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="50.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="5.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="1" max="1" width="50" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2544,13 +2441,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
@@ -2558,18 +2455,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="29.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="31.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="59.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="31.5703125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="59.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2797,29 +2694,29 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W80"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection activeCell="B2" pane="bottomLeft" sqref="B2:C4"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="24.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="43.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="43.140625" collapsed="true"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="43.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>94</v>
       </c>
@@ -2838,10 +2735,10 @@
         <v>201</v>
       </c>
       <c r="B2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C2" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -2849,7 +2746,7 @@
         <v>255</v>
       </c>
       <c r="B3" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -2870,7 +2767,7 @@
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
     </row>
-    <row customFormat="1" r="9" s="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H9" s="2"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -2921,10 +2818,10 @@
       <c r="U21" s="31"/>
       <c r="V21" s="31"/>
     </row>
-    <row customFormat="1" r="26" s="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H26" s="2"/>
     </row>
-    <row customFormat="1" r="32" s="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H32" s="2"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
@@ -2969,13 +2866,13 @@
       <c r="R42" s="4"/>
       <c r="S42" s="4"/>
     </row>
-    <row customFormat="1" r="47" s="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G47" s="2"/>
     </row>
-    <row customFormat="1" r="52" s="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G52" s="2"/>
     </row>
-    <row customFormat="1" r="57" s="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H57" s="2"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
@@ -3032,7 +2929,7 @@
       <c r="O73" s="4"/>
       <c r="P73" s="4"/>
     </row>
-    <row customFormat="1" r="80" s="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G80" s="2"/>
     </row>
   </sheetData>
@@ -3040,13 +2937,13 @@
     <mergeCell ref="A14:V14"/>
     <mergeCell ref="A21:V21"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:D6"/>
@@ -3054,13 +2951,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="46.42578125" collapsed="true"/>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="46.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>94</v>
       </c>
@@ -3079,13 +2976,13 @@
         <v>202</v>
       </c>
       <c r="B2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C2" t="s">
         <v>318</v>
       </c>
-      <c r="C2" t="s">
-        <v>321</v>
-      </c>
       <c r="D2" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -3093,10 +2990,10 @@
         <v>250</v>
       </c>
       <c r="B3" t="s">
+        <v>317</v>
+      </c>
+      <c r="C3" t="s">
         <v>320</v>
-      </c>
-      <c r="C3" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -3116,17 +3013,17 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
     </row>
-    <row customFormat="1" r="9" s="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D9" s="2"/>
     </row>
-    <row customFormat="1" r="15" s="2" spans="1:15" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="20" s="4" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="4:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D20" s="2"/>
     </row>
-    <row customFormat="1" r="25" s="4" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F25" s="2"/>
     </row>
-    <row customFormat="1" r="32" s="4" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F32" s="2"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -3167,16 +3064,16 @@
       <c r="O42" s="4"/>
       <c r="P42" s="4"/>
     </row>
-    <row customFormat="1" r="47" s="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E47" s="2"/>
     </row>
-    <row customFormat="1" r="52" s="4" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E52" s="2"/>
     </row>
-    <row customFormat="1" r="57" s="4" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D57" s="2"/>
     </row>
-    <row customFormat="1" r="62" s="4" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D62" s="2"/>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
@@ -3217,67 +3114,67 @@
       <c r="P73" s="4"/>
       <c r="Q73" s="4"/>
     </row>
-    <row customFormat="1" r="81" s="4" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E81" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AS81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="R1" sqref="R1"/>
-      <selection activeCell="A17" pane="bottomLeft" sqref="A17:N17"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="37.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="27.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="27.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="27.7109375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="29.42578125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
-    <col min="22" max="24" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="27" max="27" width="9.140625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="35" max="35" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="36" max="36" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="37" max="37" customWidth="true" style="10" width="15.0" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="98.7109375" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="37.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="27.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="27.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="27.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="29.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="24" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.140625" collapsed="1"/>
+    <col min="28" max="28" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="15" style="10" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="30.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="98.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>94</v>
       </c>
@@ -3410,16 +3307,13 @@
         <v>142</v>
       </c>
       <c r="C2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D2" t="s">
-        <v>318</v>
-      </c>
-      <c r="E2" t="s">
-        <v>348</v>
+        <v>315</v>
       </c>
       <c r="F2" t="s">
-        <v>107</v>
+        <v>204</v>
       </c>
       <c r="J2" t="s">
         <v>275</v>
@@ -3434,7 +3328,7 @@
         <v>274</v>
       </c>
       <c r="AN2" t="s">
-        <v>359</v>
+        <v>333</v>
       </c>
       <c r="AO2" t="s">
         <v>301</v>
@@ -3448,25 +3342,22 @@
         <v>142</v>
       </c>
       <c r="C3" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D3" t="s">
-        <v>318</v>
-      </c>
-      <c r="E3" t="s">
-        <v>349</v>
+        <v>315</v>
       </c>
       <c r="F3" t="s">
-        <v>107</v>
+        <v>204</v>
       </c>
       <c r="AN3" t="s">
-        <v>366</v>
+        <v>337</v>
       </c>
       <c r="AO3" t="s">
         <v>301</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.25" r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>252</v>
       </c>
@@ -3474,19 +3365,16 @@
         <v>142</v>
       </c>
       <c r="C4" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D4" t="s">
-        <v>318</v>
-      </c>
-      <c r="E4" t="s">
-        <v>350</v>
+        <v>315</v>
       </c>
       <c r="F4" t="s">
         <v>204</v>
       </c>
     </row>
-    <row ht="14.25" r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -3505,19 +3393,19 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
     </row>
-    <row ht="14.25" r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" ht="14.25" x14ac:dyDescent="0.25">
       <c r="AL7" s="11"/>
     </row>
-    <row ht="14.25" r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" ht="14.25" x14ac:dyDescent="0.25">
       <c r="AK9"/>
     </row>
-    <row customFormat="1" ht="14.25" r="10" s="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="F10" s="2"/>
     </row>
-    <row ht="14.25" r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" ht="14.25" x14ac:dyDescent="0.25">
       <c r="AK11" s="12"/>
     </row>
-    <row ht="14.25" r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" ht="14.25" x14ac:dyDescent="0.25">
       <c r="AK14"/>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
@@ -3542,13 +3430,13 @@
       <c r="M17" s="32"/>
       <c r="N17" s="32"/>
     </row>
-    <row customFormat="1" r="23" s="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F23" s="2"/>
     </row>
-    <row customFormat="1" r="28" s="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F28" s="2"/>
     </row>
-    <row customFormat="1" r="34" s="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:45" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F34" s="2"/>
     </row>
     <row r="39" spans="1:45" x14ac:dyDescent="0.25">
@@ -3562,7 +3450,7 @@
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
     </row>
-    <row customFormat="1" r="43" s="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:45" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E43" s="2"/>
     </row>
     <row r="48" spans="1:45" x14ac:dyDescent="0.25">
@@ -3821,52 +3709,52 @@
       <c r="AR68" s="4"/>
       <c r="AS68" s="4"/>
     </row>
-    <row customFormat="1" r="78" s="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:45" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F78" s="2"/>
       <c r="AK78" s="13"/>
     </row>
-    <row customHeight="1" ht="19.5" r="79" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:45" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AK79"/>
     </row>
     <row r="80" spans="1:45" x14ac:dyDescent="0.25">
       <c r="AK80"/>
     </row>
-    <row customFormat="1" r="81" x14ac:dyDescent="0.25"/>
+    <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A17:N17"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CM76"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CL76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection activeCell="G9" activeCellId="1" pane="bottomLeft" sqref="D18 G9"/>
+      <selection pane="bottomLeft" activeCell="G9" activeCellId="1" sqref="D18 G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="36.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="24.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="36" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="9" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:90" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>94</v>
       </c>
@@ -3909,7 +3797,7 @@
         <v>205</v>
       </c>
       <c r="B2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C2" t="s">
         <v>206</v>
@@ -4028,10 +3916,10 @@
       <c r="CK5" s="4"/>
       <c r="CL5" s="4"/>
     </row>
-    <row customFormat="1" r="9" s="4" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:90" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H9" s="2"/>
     </row>
-    <row customFormat="1" r="15" s="4" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:90" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -4052,14 +3940,14 @@
       <c r="S15" s="14"/>
       <c r="T15" s="14"/>
     </row>
-    <row customFormat="1" r="20" s="4" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row customFormat="1" r="26" s="4" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F26" s="2"/>
     </row>
-    <row customFormat="1" r="30" s="4" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F30" s="2"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -4088,16 +3976,16 @@
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
     </row>
-    <row customFormat="1" r="50" s="4" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E50" s="2"/>
     </row>
-    <row customFormat="1" r="55" s="4" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E55" s="2"/>
     </row>
-    <row customFormat="1" r="60" s="4" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H60" s="2"/>
     </row>
-    <row customFormat="1" r="64" s="4" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H64" s="2"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
@@ -4126,32 +4014,32 @@
       <c r="J71" s="4"/>
       <c r="K71" s="4"/>
     </row>
-    <row customFormat="1" r="76" s="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F76" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R85"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="B2" pane="bottomLeft" sqref="B2:D4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="25.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>94</v>
       </c>
@@ -4170,13 +4058,13 @@
         <v>210</v>
       </c>
       <c r="B2" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -4184,13 +4072,13 @@
         <v>253</v>
       </c>
       <c r="B3" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C3" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D3" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -4210,15 +4098,15 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
     </row>
-    <row customFormat="1" r="9" s="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E9" s="2"/>
     </row>
-    <row customFormat="1" r="17" s="2" spans="8:8" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="23" s="2" spans="8:8" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="29" s="4" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:8" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="8:8" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="8:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H29" s="2"/>
     </row>
-    <row customFormat="1" r="35" s="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H35" s="2"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -4257,16 +4145,16 @@
       <c r="N47" s="4"/>
       <c r="O47" s="4"/>
     </row>
-    <row customFormat="1" r="52" s="4" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E52" s="2"/>
     </row>
-    <row customFormat="1" r="58" s="4" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E58" s="2"/>
     </row>
-    <row customFormat="1" r="64" s="4" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E64" s="2"/>
     </row>
-    <row customFormat="1" r="69" s="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E69" s="2"/>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.25">
@@ -4307,17 +4195,17 @@
       <c r="P79" s="4"/>
       <c r="Q79" s="4"/>
     </row>
-    <row customFormat="1" r="85" s="4" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D85" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T68"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C2"/>
@@ -4325,12 +4213,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>94</v>
       </c>
@@ -4346,10 +4234,10 @@
         <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -4372,19 +4260,19 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
     </row>
-    <row customFormat="1" r="9" s="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F9" s="2"/>
     </row>
-    <row customFormat="1" r="14" s="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F14" s="2"/>
     </row>
-    <row customFormat="1" r="18" s="4" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F18" s="2"/>
     </row>
-    <row customFormat="1" r="22" s="4" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F22" s="2"/>
     </row>
-    <row customFormat="1" r="29" s="4" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F29" s="2"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
@@ -4428,35 +4316,35 @@
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
     </row>
-    <row customFormat="1" r="43" s="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H43" s="2"/>
     </row>
-    <row customFormat="1" r="47" s="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H47" s="2"/>
     </row>
-    <row customFormat="1" r="52" s="4" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="6:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F52" s="2"/>
     </row>
-    <row customFormat="1" r="56" s="4" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="6:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F56" s="2"/>
     </row>
-    <row customFormat="1" r="60" s="4" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="6:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F60" s="2"/>
     </row>
-    <row customFormat="1" r="64" s="4" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="6:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F64" s="2"/>
     </row>
-    <row customFormat="1" r="68" s="4" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="6:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F68" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R84"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C3"/>
@@ -4464,13 +4352,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>94</v>
       </c>
@@ -4489,13 +4377,13 @@
         <v>212</v>
       </c>
       <c r="B2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D2" t="s">
-        <v>351</v>
+        <v>329</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -4503,13 +4391,13 @@
         <v>254</v>
       </c>
       <c r="B3" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D3" t="s">
         <v>330</v>
-      </c>
-      <c r="D3" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -4526,19 +4414,19 @@
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
     </row>
-    <row customFormat="1" r="9" s="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D9" s="2"/>
     </row>
-    <row customFormat="1" r="17" s="4" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D17" s="2"/>
     </row>
-    <row customFormat="1" r="22" s="4" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D22" s="2"/>
     </row>
-    <row customFormat="1" r="28" s="4" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F28" s="2"/>
     </row>
-    <row customFormat="1" r="35" s="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D35" s="2"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -4575,74 +4463,74 @@
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
     </row>
-    <row customFormat="1" r="52" s="4" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E52" s="2"/>
     </row>
-    <row customFormat="1" r="57" s="4" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E57" s="2"/>
     </row>
-    <row customFormat="1" r="63" s="4" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D63" s="2"/>
     </row>
-    <row customFormat="1" r="68" s="4" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D68" s="2"/>
     </row>
-    <row customFormat="1" r="73" s="4" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F73" s="2"/>
     </row>
-    <row customFormat="1" r="78" s="4" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F78" s="2"/>
     </row>
-    <row customFormat="1" r="84" s="4" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="6:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F84" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AF16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="44.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="9" max="10" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="11" max="12" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="28" max="28" width="9.140625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="27.7109375" collapsed="true"/>
-    <col min="33" max="16384" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="44.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="12" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="9.140625" collapsed="1"/>
+    <col min="29" max="29" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="27.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="16384" width="9.140625" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
@@ -4767,7 +4655,7 @@
         <v>177</v>
       </c>
       <c r="I2" s="30" t="s">
-        <v>347</v>
+        <v>328</v>
       </c>
       <c r="O2" s="7" t="s">
         <v>193</v>
@@ -4818,7 +4706,7 @@
         <v>187</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>188</v>
       </c>
@@ -4826,14 +4714,12 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D3" t="s">
-        <v>343</v>
-      </c>
-      <c r="E3" t="s">
-        <v>344</v>
-      </c>
+        <v>338</v>
+      </c>
+      <c r="E3"/>
       <c r="F3" s="7" t="s">
         <v>176</v>
       </c>
@@ -4844,7 +4730,7 @@
         <v>177</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>347</v>
+        <v>328</v>
       </c>
       <c r="J3"/>
       <c r="K3" t="s">
@@ -4893,13 +4779,10 @@
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D4" t="s">
-        <v>345</v>
-      </c>
-      <c r="E4" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="F4" t="s">
         <v>176</v>
@@ -4911,7 +4794,7 @@
         <v>177</v>
       </c>
       <c r="I4" s="30" t="s">
-        <v>347</v>
+        <v>328</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
@@ -4922,13 +4805,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D5" t="s">
-        <v>342</v>
-      </c>
-      <c r="E5" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
@@ -5102,11 +4982,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="S3"/>
-    <hyperlink r:id="rId2" ref="T3"/>
-    <hyperlink r:id="rId3" ref="R2"/>
+    <hyperlink ref="S3" r:id="rId1"/>
+    <hyperlink ref="T3" r:id="rId2"/>
+    <hyperlink ref="R2" r:id="rId3"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="200" orientation="portrait" r:id="rId4" verticalDpi="200"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Set Test Cases File
</commit_message>
<xml_diff>
--- a/SmokeTestCases.xlsx
+++ b/SmokeTestCases.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView tabRatio="587" windowHeight="11160" windowWidth="20730" xWindow="-120" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="587" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="FilePath" r:id="rId1" sheetId="2"/>
-    <sheet name="Institutions" r:id="rId2" sheetId="3"/>
-    <sheet name="Limited Partner" r:id="rId3" sheetId="11"/>
-    <sheet name="Contact" r:id="rId4" sheetId="4"/>
-    <sheet name="Funds" r:id="rId5" sheetId="5"/>
-    <sheet name="Fundraisings" r:id="rId6" sheetId="6"/>
-    <sheet name="Partnerships" r:id="rId7" sheetId="12"/>
-    <sheet name="Commitments" r:id="rId8" sheetId="13"/>
-    <sheet name="Users" r:id="rId9" sheetId="8"/>
-    <sheet name="FolderTemp" r:id="rId10" sheetId="7"/>
-    <sheet name="DR Analytics" r:id="rId11" sheetId="9"/>
-    <sheet name="SpecialChar" r:id="rId12" sheetId="10"/>
+    <sheet name="FilePath" sheetId="2" r:id="rId1"/>
+    <sheet name="Institutions" sheetId="3" r:id="rId2"/>
+    <sheet name="Limited Partner" sheetId="11" r:id="rId3"/>
+    <sheet name="Contact" sheetId="4" r:id="rId4"/>
+    <sheet name="Funds" sheetId="5" r:id="rId5"/>
+    <sheet name="Fundraisings" sheetId="6" r:id="rId6"/>
+    <sheet name="Partnerships" sheetId="12" r:id="rId7"/>
+    <sheet name="Commitments" sheetId="13" r:id="rId8"/>
+    <sheet name="Users" sheetId="8" r:id="rId9"/>
+    <sheet name="FolderTemp" sheetId="7" r:id="rId10"/>
+    <sheet name="DR Analytics" sheetId="9" r:id="rId11"/>
+    <sheet name="SpecialChar" sheetId="10" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="339">
   <si>
     <t>Internal</t>
   </si>
@@ -944,15 +944,6 @@
     <t>StandardFile1.pdf</t>
   </si>
   <si>
-    <t>CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log</t>
-  </si>
-  <si>
-    <t>SharedFile1.pdf&lt;break&gt;SharedFile2.xlsx&lt;break&gt;SharedFile3.log</t>
-  </si>
-  <si>
-    <t>StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log</t>
-  </si>
-  <si>
     <t>Smoketc012_2_updateDocumentCRMSideAndCheckDuplicatePopUp</t>
   </si>
   <si>
@@ -971,9 +962,6 @@
     <t>Smoketc030_2_updateDocumentCRMSideAndCheckDuplicatePopUp</t>
   </si>
   <si>
-    <t>Onlineimport.log&lt;break&gt;Onlineimport.xlsx&lt;break&gt;OnlineimportFile1.pdf&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log</t>
-  </si>
-  <si>
     <t>SmokeTemplate</t>
   </si>
   <si>
@@ -1025,84 +1013,15 @@
     <t>AAAP1</t>
   </si>
   <si>
-    <t>automationnavatar+89473@gmail.com</t>
-  </si>
-  <si>
-    <t>automationnavatar+61382@gmail.com</t>
-  </si>
-  <si>
-    <t>CMT - 002848</t>
-  </si>
-  <si>
-    <t>CMT - 002849</t>
-  </si>
-  <si>
-    <t>CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log</t>
-  </si>
-  <si>
-    <t>CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log</t>
-  </si>
-  <si>
-    <t>SharedFile1.pdf&lt;break&gt;SharedFile2.xlsx&lt;break&gt;SharedFile3.log&lt;break&gt;SharedFile1.pdf&lt;break&gt;SharedFile2.xlsx&lt;break&gt;SharedFile3.log&lt;break&gt;SharedFile1.pdf&lt;break&gt;SharedFile2.xlsx&lt;break&gt;SharedFile3.log&lt;break&gt;SharedFile1.pdf&lt;break&gt;SharedFile2.xlsx&lt;break&gt;SharedFile3.log</t>
-  </si>
-  <si>
-    <t>StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log</t>
-  </si>
-  <si>
-    <t>CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log</t>
-  </si>
-  <si>
-    <t>automationnavatar+68493@gmail.com</t>
-  </si>
-  <si>
-    <t>navatariptesting+51753@gmail.com</t>
-  </si>
-  <si>
-    <t>User19353</t>
-  </si>
-  <si>
-    <t>User6874</t>
-  </si>
-  <si>
-    <t>navatariptesting+88869@gmail.com</t>
-  </si>
-  <si>
-    <t>User81019</t>
-  </si>
-  <si>
-    <t>navatariptesting+60456@gmail.com</t>
-  </si>
-  <si>
     <t>petrial4440</t>
   </si>
   <si>
-    <t>automationnavatar+13150@gmail.com</t>
-  </si>
-  <si>
-    <t>automationnavatar+35014@gmail.com</t>
-  </si>
-  <si>
-    <t>automationnavatar+3670@gmail.com</t>
-  </si>
-  <si>
     <t>CMT - 000932</t>
   </si>
   <si>
     <t>CMT - 000933</t>
   </si>
   <si>
-    <t>CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log</t>
-  </si>
-  <si>
-    <t>SharedFile1.pdf&lt;break&gt;SharedFile2.xlsx&lt;break&gt;SharedFile3.log&lt;break&gt;SharedFile1.pdf&lt;break&gt;SharedFile2.xlsx&lt;break&gt;SharedFile3.log&lt;break&gt;SharedFile1.pdf&lt;break&gt;SharedFile2.xlsx&lt;break&gt;SharedFile3.log&lt;break&gt;SharedFile1.pdf&lt;break&gt;SharedFile2.xlsx&lt;break&gt;SharedFile3.log&lt;break&gt;SharedFile1.pdf&lt;break&gt;SharedFile2.xlsx&lt;break&gt;SharedFile3.log</t>
-  </si>
-  <si>
-    <t>StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log</t>
-  </si>
-  <si>
-    <t>CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log</t>
-  </si>
-  <si>
     <t>CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log</t>
   </si>
   <si>
@@ -1118,26 +1037,22 @@
     <t>StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log</t>
   </si>
   <si>
-    <t>CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log</t>
-  </si>
-  <si>
     <t>CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log&lt;break&gt;CommonFile1.pdf&lt;break&gt;CommonFile2.xlsx&lt;break&gt;CommonFile3.log</t>
   </si>
   <si>
-    <t>Onlineimport.log&lt;break&gt;Onlineimport.xlsx&lt;break&gt;OnlineimportFile1.pdf&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log</t>
-  </si>
-  <si>
     <t>Onlineimport.log&lt;break&gt;Onlineimport.xlsx&lt;break&gt;OnlineimportFile1.pdf&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log&lt;break&gt;StandardFile1.pdf&lt;break&gt;StandardFile2.xlsx&lt;break&gt;StandardFile3.log</t>
   </si>
   <si>
     <t>http://dtaghub03.secure.force.com/apex/ResetPassword?userId=MDA1NmcwMDAwMDVBbGlGQUFT</t>
+  </si>
+  <si>
+    <t>User</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1233,78 +1148,78 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="33">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="1"/>
-    <xf applyBorder="1" applyFill="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1321,10 +1236,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1359,7 +1274,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1394,7 +1309,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1488,21 +1403,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1519,7 +1434,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1571,48 +1486,48 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK105"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AJ105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="65.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="103.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="57.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="53.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="103.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="255.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="115.5703125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="46.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="33.42578125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="52.7109375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="224.140625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="209.28515625" collapsed="true"/>
+    <col min="1" max="1" width="65.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="103.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="57.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="53.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="103.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="255.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="115.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="46.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="33.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="52.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="224.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="209.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>95</v>
       </c>
@@ -1730,7 +1645,7 @@
         <v>2</v>
       </c>
     </row>
-    <row ht="15.75" r="3" spans="1:36" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>257</v>
       </c>
@@ -1738,7 +1653,7 @@
         <v>217</v>
       </c>
     </row>
-    <row customFormat="1" ht="15.75" r="4" s="7" spans="1:36" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>259</v>
       </c>
@@ -1770,18 +1685,6 @@
       <c r="E6" t="s">
         <v>2</v>
       </c>
-      <c r="F6" t="s">
-        <v>353</v>
-      </c>
-      <c r="H6" t="s">
-        <v>354</v>
-      </c>
-      <c r="I6" t="s">
-        <v>355</v>
-      </c>
-      <c r="J6" t="s">
-        <v>304</v>
-      </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1799,7 +1702,7 @@
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E8" t="s">
         <v>2</v>
@@ -1810,7 +1713,7 @@
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B9" t="s">
         <v>215</v>
@@ -1819,13 +1722,13 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>357</v>
+        <v>330</v>
       </c>
       <c r="I9" t="s">
         <v>266</v>
       </c>
       <c r="J9" t="s">
-        <v>358</v>
+        <v>331</v>
       </c>
       <c r="N9" t="s">
         <v>267</v>
@@ -1935,14 +1838,8 @@
       <c r="E18" t="s">
         <v>2</v>
       </c>
-      <c r="F18" t="s">
-        <v>309</v>
-      </c>
       <c r="H18" t="s">
-        <v>360</v>
-      </c>
-      <c r="I18" t="s">
-        <v>361</v>
+        <v>333</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
@@ -1961,7 +1858,7 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="E20" t="s">
         <v>2</v>
@@ -1972,7 +1869,7 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B21" t="s">
         <v>215</v>
@@ -1981,16 +1878,16 @@
         <v>2</v>
       </c>
       <c r="F21" t="s">
-        <v>363</v>
+        <v>335</v>
       </c>
       <c r="I21" t="s">
-        <v>365</v>
+        <v>336</v>
       </c>
       <c r="J21" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="M21" t="s">
-        <v>361</v>
+        <v>334</v>
       </c>
       <c r="N21" t="s">
         <v>267</v>
@@ -2094,7 +1991,7 @@
         <v>303</v>
       </c>
       <c r="AE28" s="7" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
@@ -2326,13 +2223,13 @@
       <c r="A105" s="3"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
@@ -2340,25 +2237,25 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="77.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="5" max="10" width="9.140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="9.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="255.7109375" collapsed="true"/>
-    <col min="13" max="16384" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="77.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="10" width="9.140625" collapsed="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="255.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="9.140625" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>213</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row customFormat="1" r="2" s="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -2453,14 +2350,14 @@
       <c r="L8" s="22"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
@@ -2468,9 +2365,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="50.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="5.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="1" max="1" width="50" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2544,13 +2441,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
@@ -2558,18 +2455,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="29.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="31.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="59.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="31.5703125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="59.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2797,29 +2694,29 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W80"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection activeCell="B2" pane="bottomLeft" sqref="B2:C4"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="24.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="43.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="43.140625" collapsed="true"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="43.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>94</v>
       </c>
@@ -2838,10 +2735,10 @@
         <v>201</v>
       </c>
       <c r="B2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C2" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -2849,7 +2746,7 @@
         <v>255</v>
       </c>
       <c r="B3" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -2870,7 +2767,7 @@
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
     </row>
-    <row customFormat="1" r="9" s="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H9" s="2"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -2921,10 +2818,10 @@
       <c r="U21" s="31"/>
       <c r="V21" s="31"/>
     </row>
-    <row customFormat="1" r="26" s="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H26" s="2"/>
     </row>
-    <row customFormat="1" r="32" s="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H32" s="2"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
@@ -2969,13 +2866,13 @@
       <c r="R42" s="4"/>
       <c r="S42" s="4"/>
     </row>
-    <row customFormat="1" r="47" s="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G47" s="2"/>
     </row>
-    <row customFormat="1" r="52" s="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G52" s="2"/>
     </row>
-    <row customFormat="1" r="57" s="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H57" s="2"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
@@ -3032,7 +2929,7 @@
       <c r="O73" s="4"/>
       <c r="P73" s="4"/>
     </row>
-    <row customFormat="1" r="80" s="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G80" s="2"/>
     </row>
   </sheetData>
@@ -3040,13 +2937,13 @@
     <mergeCell ref="A14:V14"/>
     <mergeCell ref="A21:V21"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:D6"/>
@@ -3054,13 +2951,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="46.42578125" collapsed="true"/>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="46.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>94</v>
       </c>
@@ -3079,13 +2976,13 @@
         <v>202</v>
       </c>
       <c r="B2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D2" t="s">
         <v>318</v>
-      </c>
-      <c r="C2" t="s">
-        <v>321</v>
-      </c>
-      <c r="D2" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -3093,10 +2990,10 @@
         <v>250</v>
       </c>
       <c r="B3" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C3" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -3116,17 +3013,17 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
     </row>
-    <row customFormat="1" r="9" s="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D9" s="2"/>
     </row>
-    <row customFormat="1" r="15" s="2" spans="1:15" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="20" s="4" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="4:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D20" s="2"/>
     </row>
-    <row customFormat="1" r="25" s="4" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F25" s="2"/>
     </row>
-    <row customFormat="1" r="32" s="4" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F32" s="2"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -3167,16 +3064,16 @@
       <c r="O42" s="4"/>
       <c r="P42" s="4"/>
     </row>
-    <row customFormat="1" r="47" s="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E47" s="2"/>
     </row>
-    <row customFormat="1" r="52" s="4" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E52" s="2"/>
     </row>
-    <row customFormat="1" r="57" s="4" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D57" s="2"/>
     </row>
-    <row customFormat="1" r="62" s="4" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D62" s="2"/>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
@@ -3217,67 +3114,67 @@
       <c r="P73" s="4"/>
       <c r="Q73" s="4"/>
     </row>
-    <row customFormat="1" r="81" s="4" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E81" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AS81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="R1" sqref="R1"/>
-      <selection activeCell="A17" pane="bottomLeft" sqref="A17:N17"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="37.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="27.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="27.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="27.7109375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="29.42578125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
-    <col min="22" max="24" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="27" max="27" width="9.140625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="35" max="35" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="36" max="36" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="37" max="37" customWidth="true" style="10" width="15.0" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="98.7109375" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="37.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="27.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="27.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="27.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="29.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="24" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.140625" collapsed="1"/>
+    <col min="28" max="28" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="15" style="10" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="30.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="98.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>94</v>
       </c>
@@ -3410,16 +3307,13 @@
         <v>142</v>
       </c>
       <c r="C2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D2" t="s">
-        <v>318</v>
-      </c>
-      <c r="E2" t="s">
-        <v>348</v>
+        <v>314</v>
       </c>
       <c r="F2" t="s">
-        <v>107</v>
+        <v>204</v>
       </c>
       <c r="J2" t="s">
         <v>275</v>
@@ -3434,7 +3328,7 @@
         <v>274</v>
       </c>
       <c r="AN2" t="s">
-        <v>359</v>
+        <v>332</v>
       </c>
       <c r="AO2" t="s">
         <v>301</v>
@@ -3448,25 +3342,22 @@
         <v>142</v>
       </c>
       <c r="C3" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D3" t="s">
-        <v>318</v>
-      </c>
-      <c r="E3" t="s">
-        <v>349</v>
+        <v>314</v>
       </c>
       <c r="F3" t="s">
-        <v>107</v>
+        <v>204</v>
       </c>
       <c r="AN3" t="s">
-        <v>366</v>
+        <v>337</v>
       </c>
       <c r="AO3" t="s">
         <v>301</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.25" r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>252</v>
       </c>
@@ -3474,19 +3365,16 @@
         <v>142</v>
       </c>
       <c r="C4" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D4" t="s">
-        <v>318</v>
-      </c>
-      <c r="E4" t="s">
-        <v>350</v>
+        <v>314</v>
       </c>
       <c r="F4" t="s">
         <v>204</v>
       </c>
     </row>
-    <row ht="14.25" r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -3505,19 +3393,19 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
     </row>
-    <row ht="14.25" r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" ht="14.25" x14ac:dyDescent="0.25">
       <c r="AL7" s="11"/>
     </row>
-    <row ht="14.25" r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" ht="14.25" x14ac:dyDescent="0.25">
       <c r="AK9"/>
     </row>
-    <row customFormat="1" ht="14.25" r="10" s="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="F10" s="2"/>
     </row>
-    <row ht="14.25" r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" ht="14.25" x14ac:dyDescent="0.25">
       <c r="AK11" s="12"/>
     </row>
-    <row ht="14.25" r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" ht="14.25" x14ac:dyDescent="0.25">
       <c r="AK14"/>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
@@ -3542,13 +3430,13 @@
       <c r="M17" s="32"/>
       <c r="N17" s="32"/>
     </row>
-    <row customFormat="1" r="23" s="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F23" s="2"/>
     </row>
-    <row customFormat="1" r="28" s="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F28" s="2"/>
     </row>
-    <row customFormat="1" r="34" s="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:45" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F34" s="2"/>
     </row>
     <row r="39" spans="1:45" x14ac:dyDescent="0.25">
@@ -3562,7 +3450,7 @@
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
     </row>
-    <row customFormat="1" r="43" s="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:45" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E43" s="2"/>
     </row>
     <row r="48" spans="1:45" x14ac:dyDescent="0.25">
@@ -3821,52 +3709,52 @@
       <c r="AR68" s="4"/>
       <c r="AS68" s="4"/>
     </row>
-    <row customFormat="1" r="78" s="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:45" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F78" s="2"/>
       <c r="AK78" s="13"/>
     </row>
-    <row customHeight="1" ht="19.5" r="79" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:45" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AK79"/>
     </row>
     <row r="80" spans="1:45" x14ac:dyDescent="0.25">
       <c r="AK80"/>
     </row>
-    <row customFormat="1" r="81" x14ac:dyDescent="0.25"/>
+    <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A17:N17"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CM76"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CL76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection activeCell="G9" activeCellId="1" pane="bottomLeft" sqref="D18 G9"/>
+      <selection pane="bottomLeft" activeCell="G9" activeCellId="1" sqref="D18 G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="36.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="24.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="36" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="9" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:90" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>94</v>
       </c>
@@ -3909,7 +3797,7 @@
         <v>205</v>
       </c>
       <c r="B2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C2" t="s">
         <v>206</v>
@@ -4028,10 +3916,10 @@
       <c r="CK5" s="4"/>
       <c r="CL5" s="4"/>
     </row>
-    <row customFormat="1" r="9" s="4" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:90" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H9" s="2"/>
     </row>
-    <row customFormat="1" r="15" s="4" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:90" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -4052,14 +3940,14 @@
       <c r="S15" s="14"/>
       <c r="T15" s="14"/>
     </row>
-    <row customFormat="1" r="20" s="4" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row customFormat="1" r="26" s="4" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F26" s="2"/>
     </row>
-    <row customFormat="1" r="30" s="4" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F30" s="2"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -4088,16 +3976,16 @@
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
     </row>
-    <row customFormat="1" r="50" s="4" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E50" s="2"/>
     </row>
-    <row customFormat="1" r="55" s="4" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E55" s="2"/>
     </row>
-    <row customFormat="1" r="60" s="4" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H60" s="2"/>
     </row>
-    <row customFormat="1" r="64" s="4" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H64" s="2"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
@@ -4126,32 +4014,32 @@
       <c r="J71" s="4"/>
       <c r="K71" s="4"/>
     </row>
-    <row customFormat="1" r="76" s="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F76" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R85"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="B2" pane="bottomLeft" sqref="B2:D4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="25.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>94</v>
       </c>
@@ -4170,13 +4058,13 @@
         <v>210</v>
       </c>
       <c r="B2" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -4184,13 +4072,13 @@
         <v>253</v>
       </c>
       <c r="B3" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C3" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="D3" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -4210,15 +4098,15 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
     </row>
-    <row customFormat="1" r="9" s="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E9" s="2"/>
     </row>
-    <row customFormat="1" r="17" s="2" spans="8:8" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="23" s="2" spans="8:8" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="29" s="4" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:8" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="8:8" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="8:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H29" s="2"/>
     </row>
-    <row customFormat="1" r="35" s="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H35" s="2"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -4257,16 +4145,16 @@
       <c r="N47" s="4"/>
       <c r="O47" s="4"/>
     </row>
-    <row customFormat="1" r="52" s="4" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E52" s="2"/>
     </row>
-    <row customFormat="1" r="58" s="4" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E58" s="2"/>
     </row>
-    <row customFormat="1" r="64" s="4" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E64" s="2"/>
     </row>
-    <row customFormat="1" r="69" s="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E69" s="2"/>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.25">
@@ -4307,17 +4195,17 @@
       <c r="P79" s="4"/>
       <c r="Q79" s="4"/>
     </row>
-    <row customFormat="1" r="85" s="4" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D85" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T68"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C2"/>
@@ -4325,12 +4213,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>94</v>
       </c>
@@ -4346,10 +4234,10 @@
         <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -4372,19 +4260,19 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
     </row>
-    <row customFormat="1" r="9" s="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F9" s="2"/>
     </row>
-    <row customFormat="1" r="14" s="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F14" s="2"/>
     </row>
-    <row customFormat="1" r="18" s="4" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F18" s="2"/>
     </row>
-    <row customFormat="1" r="22" s="4" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F22" s="2"/>
     </row>
-    <row customFormat="1" r="29" s="4" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F29" s="2"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
@@ -4428,35 +4316,35 @@
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
     </row>
-    <row customFormat="1" r="43" s="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H43" s="2"/>
     </row>
-    <row customFormat="1" r="47" s="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H47" s="2"/>
     </row>
-    <row customFormat="1" r="52" s="4" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="6:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F52" s="2"/>
     </row>
-    <row customFormat="1" r="56" s="4" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="6:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F56" s="2"/>
     </row>
-    <row customFormat="1" r="60" s="4" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="6:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F60" s="2"/>
     </row>
-    <row customFormat="1" r="64" s="4" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="6:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F64" s="2"/>
     </row>
-    <row customFormat="1" r="68" s="4" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="6:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F68" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R84"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C3"/>
@@ -4464,13 +4352,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>94</v>
       </c>
@@ -4489,13 +4377,13 @@
         <v>212</v>
       </c>
       <c r="B2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C2" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D2" t="s">
-        <v>351</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -4503,13 +4391,13 @@
         <v>254</v>
       </c>
       <c r="B3" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C3" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D3" t="s">
-        <v>352</v>
+        <v>329</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -4526,19 +4414,19 @@
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
     </row>
-    <row customFormat="1" r="9" s="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D9" s="2"/>
     </row>
-    <row customFormat="1" r="17" s="4" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D17" s="2"/>
     </row>
-    <row customFormat="1" r="22" s="4" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D22" s="2"/>
     </row>
-    <row customFormat="1" r="28" s="4" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F28" s="2"/>
     </row>
-    <row customFormat="1" r="35" s="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D35" s="2"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -4575,74 +4463,74 @@
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
     </row>
-    <row customFormat="1" r="52" s="4" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E52" s="2"/>
     </row>
-    <row customFormat="1" r="57" s="4" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E57" s="2"/>
     </row>
-    <row customFormat="1" r="63" s="4" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D63" s="2"/>
     </row>
-    <row customFormat="1" r="68" s="4" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D68" s="2"/>
     </row>
-    <row customFormat="1" r="73" s="4" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F73" s="2"/>
     </row>
-    <row customFormat="1" r="78" s="4" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F78" s="2"/>
     </row>
-    <row customFormat="1" r="84" s="4" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="6:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F84" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AF16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="44.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="9" max="10" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="11" max="12" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="28" max="28" width="9.140625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="27.7109375" collapsed="true"/>
-    <col min="33" max="16384" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="44.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="12" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="9.140625" collapsed="1"/>
+    <col min="29" max="29" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="27.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="16384" width="9.140625" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
@@ -4767,7 +4655,7 @@
         <v>177</v>
       </c>
       <c r="I2" s="30" t="s">
-        <v>347</v>
+        <v>327</v>
       </c>
       <c r="O2" s="7" t="s">
         <v>193</v>
@@ -4818,7 +4706,7 @@
         <v>187</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>188</v>
       </c>
@@ -4826,14 +4714,12 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="D3" t="s">
-        <v>343</v>
-      </c>
-      <c r="E3" t="s">
-        <v>344</v>
-      </c>
+        <v>338</v>
+      </c>
+      <c r="E3"/>
       <c r="F3" s="7" t="s">
         <v>176</v>
       </c>
@@ -4844,7 +4730,7 @@
         <v>177</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>347</v>
+        <v>327</v>
       </c>
       <c r="J3"/>
       <c r="K3" t="s">
@@ -4893,13 +4779,10 @@
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D4" t="s">
-        <v>345</v>
-      </c>
-      <c r="E4" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="F4" t="s">
         <v>176</v>
@@ -4911,7 +4794,7 @@
         <v>177</v>
       </c>
       <c r="I4" s="30" t="s">
-        <v>347</v>
+        <v>327</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
@@ -4922,13 +4805,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D5" t="s">
-        <v>342</v>
-      </c>
-      <c r="E5" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
@@ -5102,11 +4982,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="S3"/>
-    <hyperlink r:id="rId2" ref="T3"/>
-    <hyperlink r:id="rId3" ref="R2"/>
+    <hyperlink ref="S3" r:id="rId1"/>
+    <hyperlink ref="T3" r:id="rId2"/>
+    <hyperlink ref="R2" r:id="rId3"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="200" orientation="portrait" r:id="rId4" verticalDpi="200"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>